<commit_message>
updated files for unit testing
</commit_message>
<xml_diff>
--- a/TextToSpeech/Resources/InputSamples/ExcelSampleSaveRot13.xlsx
+++ b/TextToSpeech/Resources/InputSamples/ExcelSampleSaveRot13.xlsx
@@ -14,40 +14,40 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
-    <t>xlofnm0</t>
+    <t>pbyhza0</t>
   </si>
   <si>
-    <t>xlofnm1</t>
+    <t>pbyhza1</t>
   </si>
   <si>
-    <t>xlofnm2</t>
+    <t>pbyhza2</t>
   </si>
   <si>
-    <t>ild1</t>
+    <t>ebj1</t>
   </si>
   <si>
-    <t>ild1 xlo1</t>
+    <t>ebj1 pby1</t>
   </si>
   <si>
-    <t>ild1 xlo2</t>
+    <t>ebj1 pby2</t>
   </si>
   <si>
-    <t>ild2</t>
+    <t>ebj2</t>
   </si>
   <si>
-    <t>ild2 xlo1</t>
+    <t>ebj2 pby1</t>
   </si>
   <si>
-    <t>ild2 xlo2</t>
+    <t>ebj2 pby2</t>
   </si>
   <si>
-    <t>ild3</t>
+    <t>ebj3</t>
   </si>
   <si>
-    <t>ild3 xlo1</t>
+    <t>ebj3 pby1</t>
   </si>
   <si>
-    <t>ild3 xlo2</t>
+    <t>ebj3 pby2</t>
   </si>
 </sst>
 </file>

</xml_diff>